<commit_message>
Made changed to iniall application by adding the upload queue sequence
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/jayalakshmi_anand_uipath_com/Documents/Documents/UiPath/ADT_Training/Jan_23_ADTbyJaya/BuisnessException_Test/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C96B18B-5C49-4B29-A305-AD44A1A73A3A}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB97EAA1-DF07-414E-8A2E-9BA5D1645F53}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,13 +160,25 @@
   </si>
   <si>
     <t>BusinessException_Test</t>
+  </si>
+  <si>
+    <t>Acme_Cred</t>
+  </si>
+  <si>
+    <t>acme cred</t>
+  </si>
+  <si>
+    <t>Acme_url</t>
+  </si>
+  <si>
+    <t>acme website_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +202,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF464E55"/>
+      <name val="Noto Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,6 +239,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,6 +255,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -537,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -615,7 +638,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2782,7 +2812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2828,7 +2860,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>